<commit_message>
Fix logging and command keys
Pair programmed with Akram
</commit_message>
<xml_diff>
--- a/resources/SPGeTTi_messages.xlsx
+++ b/resources/SPGeTTi_messages.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repository\se761\761_ChatBot\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\761_ChatBot\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13275" activeTab="3" xr2:uid="{5D90C3B8-1318-4920-AB27-7B71E2B74046}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13275" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Welcome_Messages" sheetId="1" r:id="rId1"/>
@@ -309,15 +309,6 @@
     <t>Alright, that's fine! See you later.</t>
   </si>
   <si>
-    <t>^(?=.*\\bgoals?\\b.*).*$</t>
-  </si>
-  <si>
-    <t>^(?=.*\\byes\\b.*).*$</t>
-  </si>
-  <si>
-    <t>^(?=.*\\bno\\b.*).*$</t>
-  </si>
-  <si>
     <t>^.*$</t>
   </si>
   <si>
@@ -336,20 +327,29 @@
     <t>echo</t>
   </si>
   <si>
-    <t>Great, there's lots of benefits by not gambling.\\n\\nSome benefits are getting out of debt, improving relationships, feeling healthier and less stressed, feeling better about yourself.\\n\\nWhat do you see as your benefits by stopping gambling?</t>
-  </si>
-  <si>
-    <t>Great, here are some quick tips to start this journey:\\n- Avoid tempting environments\\n- Limit access to finances\\n- Find healthier activities to do</t>
-  </si>
-  <si>
-    <t>Try to limit how many days you go gambling, or set a maximum amount you can spend.\\nTake some time now to write down what you want to achieve</t>
+    <t>Great, there's lots of benefits by not gambling.  Some benefits are getting out of debt, improving relationships, feeling healthier and less stressed, feeling better about yourself.  What do you see as your benefits by stopping gambling?</t>
+  </si>
+  <si>
+    <t>Great, here are some quick tips to start this journey:  Avoid tempting environments; Limit access to finances; Find healthier activities to do</t>
+  </si>
+  <si>
+    <t>Try to limit how many days you go gambling, or set a maximum amount you can spend.  Take some time now to write down what you want to achieve</t>
+  </si>
+  <si>
+    <t>^(?=.*\byes\b.*).*$</t>
+  </si>
+  <si>
+    <t>^(?=.*\bno\b.*).*$</t>
+  </si>
+  <si>
+    <t>^(?=.*\bgoals?\b.*).*$</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -781,20 +781,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70394DA9-4A2F-4FFB-A70B-55F5D6305C57}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -802,7 +802,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -810,7 +810,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -818,7 +818,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -826,7 +826,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -834,7 +834,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -842,7 +842,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -850,7 +850,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -858,7 +858,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -866,7 +866,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -874,7 +874,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -882,7 +882,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -897,20 +897,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EDD06DF-9923-419A-85A0-979585611EAE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.7109375" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -924,7 +924,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="36.75">
+    <row r="2" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
@@ -938,7 +938,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="36">
+    <row r="3" spans="1:4" ht="36" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>25</v>
       </c>
@@ -952,7 +952,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="36.75">
+    <row r="4" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>26</v>
       </c>
@@ -966,7 +966,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="48">
+    <row r="5" spans="1:4" ht="48" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>28</v>
       </c>
@@ -980,7 +980,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="36">
+    <row r="6" spans="1:4" ht="36" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>29</v>
       </c>
@@ -994,7 +994,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="36.75">
+    <row r="7" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>30</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="36.75">
+    <row r="8" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="36.75">
+    <row r="9" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -1036,7 +1036,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="48.75">
+    <row r="10" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="36">
+    <row r="11" spans="1:4" ht="36" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>34</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="48">
+    <row r="12" spans="1:4" ht="48" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>35</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="24">
+    <row r="13" spans="1:4" ht="24" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>36</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="36">
+    <row r="14" spans="1:4" ht="36" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>37</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="48.75">
+    <row r="15" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>39</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="48.75">
+    <row r="16" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>40</v>
       </c>
@@ -1134,7 +1134,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="36">
+    <row r="17" spans="1:4" ht="36" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>41</v>
       </c>
@@ -1148,7 +1148,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="36">
+    <row r="18" spans="1:4" ht="36" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>42</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="48">
+    <row r="19" spans="1:4" ht="48" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>43</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="48">
+    <row r="20" spans="1:4" ht="48" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>44</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="36">
+    <row r="21" spans="1:4" ht="36" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>45</v>
       </c>
@@ -1204,7 +1204,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="36.75">
+    <row r="22" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>46</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="36">
+    <row r="23" spans="1:4" ht="36" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>47</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="48.75">
+    <row r="24" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>48</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="36">
+    <row r="25" spans="1:4" ht="36" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>49</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="48.75">
+    <row r="26" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>50</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="24">
+    <row r="27" spans="1:4" ht="24" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>51</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="24">
+    <row r="28" spans="1:4" ht="24" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>52</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="36">
+    <row r="29" spans="1:4" ht="36" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>53</v>
       </c>
@@ -1316,7 +1316,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="36.75">
+    <row r="30" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>54</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="48.75">
+    <row r="31" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>55</v>
       </c>
@@ -1344,7 +1344,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="48.75">
+    <row r="32" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>56</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="48.75">
+    <row r="33" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
         <v>57</v>
       </c>
@@ -1372,7 +1372,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="48.75">
+    <row r="34" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>58</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="48.75">
+    <row r="35" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>59</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="36.75">
+    <row r="36" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>60</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="36.75">
+    <row r="37" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>61</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="36.75">
+    <row r="38" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>62</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="36">
+    <row r="39" spans="1:4" ht="36" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>63</v>
       </c>
@@ -1456,7 +1456,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="36.75">
+    <row r="40" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>64</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="48">
+    <row r="41" spans="1:4" ht="48" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>28</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="36">
+    <row r="42" spans="1:4" ht="36" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>65</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="24.75">
+    <row r="43" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>66</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="48.75">
+    <row r="44" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
         <v>67</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="48.75">
+    <row r="45" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>68</v>
       </c>
@@ -1540,7 +1540,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="24">
+    <row r="46" spans="1:4" ht="24" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>69</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="36.75">
+    <row r="47" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>70</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="24.75">
+    <row r="48" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>71</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="48">
+    <row r="49" spans="1:4" ht="48" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>72</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="36.75">
+    <row r="50" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>73</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="36.75">
+    <row r="51" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>74</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="25.5">
+    <row r="52" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>75</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="48">
+    <row r="53" spans="1:4" ht="48" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>76</v>
       </c>
@@ -1658,21 +1658,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E765B4A6-A954-42D3-A7A2-921D6B9ABE81}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>86</v>
       </c>
@@ -1689,12 +1689,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="C2" t="s">
         <v>90</v>
@@ -1713,21 +1713,21 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCB51100-5A7D-4514-8933-69E59ED41E3D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="97.42578125" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>86</v>
       </c>
@@ -1744,15 +1744,15 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="75">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
         <v>89</v>
@@ -1761,12 +1761,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C3" t="s">
         <v>92</v>
@@ -1775,63 +1775,63 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D4" t="s">
         <v>89</v>
       </c>
       <c r="E4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="45">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D6" t="s">
         <v>89</v>
       </c>
       <c r="E6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="45">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D7" t="s">
         <v>89</v>
@@ -1840,12 +1840,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C8" t="s">
         <v>92</v>
@@ -1854,15 +1854,15 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D9" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
Add input response type
Pair programmed:
 - James
 - Henry
</commit_message>
<xml_diff>
--- a/resources/SPGeTTi_messages.xlsx
+++ b/resources/SPGeTTi_messages.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13275" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13275" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Welcome_Messages" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="110">
   <si>
     <t>Country</t>
   </si>
@@ -312,18 +312,9 @@
     <t>5;6</t>
   </si>
   <si>
-    <t>echo</t>
-  </si>
-  <si>
     <t>Great, there's lots of benefits by not gambling.  Some benefits are getting out of debt, improving relationships, feeling healthier and less stressed, feeling better about yourself.  What do you see as your benefits by stopping gambling?</t>
   </si>
   <si>
-    <t>Great, here are some quick tips to start this journey:  Avoid tempting environments; Limit access to finances; Find healthier activities to do</t>
-  </si>
-  <si>
-    <t>Try to limit how many days you go gambling, or set a maximum amount you can spend.  Take some time now to write down what you want to achieve</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -343,6 +334,30 @@
   </si>
   <si>
     <t>goals</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Great, here are some quick tips to start this journey:  Avoid tempting environments; Limit access to finances; Find healthier activities to do.</t>
+  </si>
+  <si>
+    <t>Try to limit how many days you go gambling, or set a maximum amount you can spend.  Take some time now to write down what you want to achieve.</t>
+  </si>
+  <si>
+    <t>Message;Input</t>
+  </si>
+  <si>
+    <t>Benefits</t>
+  </si>
+  <si>
+    <t>Goals</t>
+  </si>
+  <si>
+    <t>Message;Buttons;Input</t>
+  </si>
+  <si>
+    <t>That’s great! I'll hold you to it.</t>
   </si>
 </sst>
 </file>
@@ -432,7 +447,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -467,6 +482,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1659,10 +1677,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1671,9 +1689,10 @@
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>85</v>
       </c>
@@ -1681,35 +1700,38 @@
         <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
         <v>87</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F2" t="s">
+        <v>100</v>
+      </c>
+      <c r="G2" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1721,21 +1743,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="97.42578125" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="96.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>85</v>
       </c>
@@ -1743,42 +1767,46 @@
         <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E2" s="12"/>
-      <c r="F2">
+      <c r="F2" s="12"/>
+      <c r="G2" s="13">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -1786,83 +1814,90 @@
       <c r="D3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="13"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="D4" t="s">
         <v>90</v>
       </c>
       <c r="E4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F4" t="s">
+        <v>106</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="E5" s="12"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="12"/>
+      <c r="G5" s="13"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" t="s">
         <v>99</v>
-      </c>
-      <c r="C6" t="s">
-        <v>102</v>
       </c>
       <c r="D6" t="s">
         <v>92</v>
       </c>
       <c r="E6" t="s">
-        <v>103</v>
-      </c>
-      <c r="F6" t="s">
+        <v>100</v>
+      </c>
+      <c r="G6" s="13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="E7" s="12"/>
-      <c r="F7">
+      <c r="F7" s="12"/>
+      <c r="G7" s="13">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
@@ -1870,20 +1905,25 @@
       <c r="D8" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>105</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="E9" s="12"/>
+      <c r="F9" s="12" t="s">
+        <v>107</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add recall response type to bot
Bot can read/recall stored information from storage (currently Google
Sheets)

Pair Programmed:
 - Henry
 - Jay
</commit_message>
<xml_diff>
--- a/resources/SPGeTTi_messages.xlsx
+++ b/resources/SPGeTTi_messages.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\761_ChatBot\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13275" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Welcome_Messages" sheetId="1" r:id="rId1"/>
@@ -17,7 +12,7 @@
     <sheet name="User_Initiated_Messages" sheetId="3" r:id="rId3"/>
     <sheet name="Follow_Up_Messages" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="114">
   <si>
     <t>Country</t>
   </si>
@@ -336,34 +331,46 @@
     <t>goals</t>
   </si>
   <si>
-    <t>Input</t>
-  </si>
-  <si>
     <t>Great, here are some quick tips to start this journey:  Avoid tempting environments; Limit access to finances; Find healthier activities to do.</t>
   </si>
   <si>
     <t>Try to limit how many days you go gambling, or set a maximum amount you can spend.  Take some time now to write down what you want to achieve.</t>
   </si>
   <si>
-    <t>Message;Input</t>
-  </si>
-  <si>
     <t>Benefits</t>
   </si>
   <si>
     <t>Goals</t>
   </si>
   <si>
-    <t>Message;Buttons;Input</t>
-  </si>
-  <si>
-    <t>That’s great! I'll hold you to it.</t>
+    <t>Message;Buttons;Store</t>
+  </si>
+  <si>
+    <t>Store</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>Message;Store</t>
+  </si>
+  <si>
+    <t>That’s great! I'll hold you to that!</t>
+  </si>
+  <si>
+    <t>my goal</t>
+  </si>
+  <si>
+    <t>Message;Recall</t>
+  </si>
+  <si>
+    <t>You set a goal of [Goals].  How is that going?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -792,7 +799,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1677,10 +1684,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1689,10 +1696,10 @@
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" customWidth="1"/>
+    <col min="6" max="7" width="7.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>85</v>
       </c>
@@ -1709,13 +1716,16 @@
         <v>98</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1731,8 +1741,25 @@
       <c r="E2" t="s">
         <v>100</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G3" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1743,9 +1770,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -1755,11 +1782,11 @@
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="96.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>85</v>
       </c>
@@ -1776,13 +1803,16 @@
         <v>98</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1797,11 +1827,12 @@
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
-      <c r="G2" s="13">
+      <c r="G2" s="12"/>
+      <c r="H2" s="13">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1814,14 +1845,14 @@
       <c r="D3" t="s">
         <v>89</v>
       </c>
-      <c r="G3" s="13"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="13"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D4" t="s">
         <v>90</v>
@@ -1830,13 +1861,13 @@
         <v>100</v>
       </c>
       <c r="F4" t="s">
-        <v>106</v>
-      </c>
-      <c r="G4" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="H4" s="13" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1847,13 +1878,14 @@
         <v>19</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
-      <c r="G5" s="13"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5" s="12"/>
+      <c r="H5" s="13"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1869,11 +1901,11 @@
       <c r="E6" t="s">
         <v>100</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="H6" s="13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1884,15 +1916,16 @@
         <v>19</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
-      <c r="G7" s="13">
+      <c r="G7" s="12"/>
+      <c r="H7" s="13">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1905,22 +1938,23 @@
       <c r="D8" t="s">
         <v>89</v>
       </c>
-      <c r="G8" s="13"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12" t="s">
-        <v>107</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="G9" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add new conversation flows as well as corresponding json files - done with John
</commit_message>
<xml_diff>
--- a/resources/SPGeTTi_messages.xlsx
+++ b/resources/SPGeTTi_messages.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\761_ChatBot\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\4th year\sem2\761\761_ChatBot\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13275" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13275" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Welcome_Messages" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="132">
   <si>
     <t>Country</t>
   </si>
@@ -343,12 +343,93 @@
   </si>
   <si>
     <t>goals</t>
+  </si>
+  <si>
+    <t>problems</t>
+  </si>
+  <si>
+    <t>Do you think you have a problem?</t>
+  </si>
+  <si>
+    <t>8;9</t>
+  </si>
+  <si>
+    <t>You are not alone. Do you want to talk to someone?</t>
+  </si>
+  <si>
+    <t>10;11</t>
+  </si>
+  <si>
+    <t>You can phone a friend, call the Gambling Helpline 0800 654 655 or text 8006 for more information</t>
+  </si>
+  <si>
+    <t>If you want more information, you can go to choicenotchance.org.nz</t>
+  </si>
+  <si>
+    <t>Do you think you can win back what you have lost by gambling more?</t>
+  </si>
+  <si>
+    <t>Do you gamble using money meant for other things?</t>
+  </si>
+  <si>
+    <t>Do you lie about your gambling to people you care about?</t>
+  </si>
+  <si>
+    <t>Do you get angry or defensive when people ask about your gambling?</t>
+  </si>
+  <si>
+    <t>Do you borrow money just so you can gamble?</t>
+  </si>
+  <si>
+    <t>Did you answer yes to most of these?</t>
+  </si>
+  <si>
+    <t>17;18</t>
+  </si>
+  <si>
+    <t>It looks like gambling is hurting you and maybe those you care about. Do you want to talk to someone about it?</t>
+  </si>
+  <si>
+    <t>Okay that's great! If you want more information, you can go to choicenotchance.org.nz</t>
+  </si>
+  <si>
+    <t>stressed</t>
+  </si>
+  <si>
+    <t>Do you need some ideas to help you relax?</t>
+  </si>
+  <si>
+    <t>19;20</t>
+  </si>
+  <si>
+    <t>Indoors;Outdoors</t>
+  </si>
+  <si>
+    <t>Do you prefer indoors or outdoors activities?</t>
+  </si>
+  <si>
+    <t>21;22</t>
+  </si>
+  <si>
+    <t>indoors</t>
+  </si>
+  <si>
+    <t>outdoors</t>
+  </si>
+  <si>
+    <t>Why don't you invite your friends over for dinner? You find some recipes at myfamily.kiwi/foods</t>
+  </si>
+  <si>
+    <t>You can go for a walk, visit a museum or gallery with your friends or family. Going to a nearby park is also a fun thing to do!</t>
+  </si>
+  <si>
+    <t>That's fine! You can always come back for more ideas if you need</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -781,7 +862,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -897,7 +978,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1658,19 +1739,19 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1711,6 +1792,46 @@
       </c>
       <c r="F2" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1720,11 +1841,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1853,9 +1974,6 @@
         <v>97</v>
       </c>
       <c r="E7" s="12"/>
-      <c r="F7">
-        <v>7</v>
-      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1882,6 +2000,255 @@
         <v>94</v>
       </c>
       <c r="E9" s="12"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D10" t="s">
+        <v>108</v>
+      </c>
+      <c r="E10" t="s">
+        <v>103</v>
+      </c>
+      <c r="F10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="E11" t="s">
+        <v>103</v>
+      </c>
+      <c r="F11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E14" t="s">
+        <v>103</v>
+      </c>
+      <c r="F14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15" t="s">
+        <v>103</v>
+      </c>
+      <c r="F15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16" t="s">
+        <v>103</v>
+      </c>
+      <c r="F16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" t="s">
+        <v>116</v>
+      </c>
+      <c r="E17" t="s">
+        <v>103</v>
+      </c>
+      <c r="F17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D18" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18" t="s">
+        <v>103</v>
+      </c>
+      <c r="F18" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" t="s">
+        <v>119</v>
+      </c>
+      <c r="E19" t="s">
+        <v>103</v>
+      </c>
+      <c r="F19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" t="s">
+        <v>125</v>
+      </c>
+      <c r="E21" t="s">
+        <v>124</v>
+      </c>
+      <c r="F21" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>127</v>
+      </c>
+      <c r="C23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>128</v>
+      </c>
+      <c r="C24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" t="s">
+        <v>130</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add example store recall messages
Pair programmed:
 - Henry
 - Jay
</commit_message>
<xml_diff>
--- a/resources/SPGeTTi_messages.xlsx
+++ b/resources/SPGeTTi_messages.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\4th year\sem2\761\761_ChatBot\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13275" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Welcome_Messages" sheetId="1" r:id="rId1"/>
@@ -17,7 +12,7 @@
     <sheet name="User_Initiated_Messages" sheetId="3" r:id="rId3"/>
     <sheet name="Follow_Up_Messages" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="140">
   <si>
     <t>Country</t>
   </si>
@@ -312,9 +307,6 @@
     <t>5;6</t>
   </si>
   <si>
-    <t>echo</t>
-  </si>
-  <si>
     <t>Great, there's lots of benefits by not gambling.  Some benefits are getting out of debt, improving relationships, feeling healthier and less stressed, feeling better about yourself.  What do you see as your benefits by stopping gambling?</t>
   </si>
   <si>
@@ -424,12 +416,39 @@
   </si>
   <si>
     <t>That's fine! You can always come back for more ideas if you need</t>
+  </si>
+  <si>
+    <t>Store</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>recall goals</t>
+  </si>
+  <si>
+    <t>Message;Recall</t>
+  </si>
+  <si>
+    <t>Your goal was: [Goals]</t>
+  </si>
+  <si>
+    <t>Goals</t>
+  </si>
+  <si>
+    <t>Message;Store</t>
+  </si>
+  <si>
+    <t>Benefits</t>
+  </si>
+  <si>
+    <t>I'll hold you to that goal!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -855,14 +874,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -978,7 +997,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1739,11 +1758,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1752,9 +1771,10 @@
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>85</v>
       </c>
@@ -1762,76 +1782,99 @@
         <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D2" t="s">
         <v>87</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F2" t="s">
+        <v>102</v>
+      </c>
+      <c r="H2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" t="s">
         <v>105</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>102</v>
       </c>
-      <c r="D3" t="s">
+      <c r="H3" t="s">
         <v>106</v>
       </c>
-      <c r="E3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" t="s">
         <v>121</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>102</v>
       </c>
-      <c r="D4" t="s">
+      <c r="H4" t="s">
         <v>122</v>
       </c>
-      <c r="E4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F4" t="s">
-        <v>123</v>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" t="s">
+        <v>135</v>
+      </c>
+      <c r="G5" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1841,11 +1884,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1853,10 +1896,10 @@
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="4" max="4" width="97.42578125" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" customWidth="1"/>
+    <col min="5" max="7" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>85</v>
       </c>
@@ -1864,42 +1907,52 @@
         <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>137</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E2" s="12"/>
-      <c r="F2">
+      <c r="F2" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -1908,79 +1961,85 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D4" t="s">
         <v>90</v>
       </c>
       <c r="E4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F4" t="s">
+        <v>102</v>
+      </c>
+      <c r="H4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E5" s="12"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D6" t="s">
         <v>92</v>
       </c>
       <c r="E6" t="s">
-        <v>103</v>
-      </c>
-      <c r="F6" t="s">
+        <v>102</v>
+      </c>
+      <c r="H6" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>137</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E7" s="12"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="G7" s="12"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
@@ -1989,7 +2048,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1997,257 +2056,259 @@
         <v>19</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>94</v>
+        <v>139</v>
       </c>
       <c r="E9" s="12"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" t="s">
         <v>102</v>
       </c>
-      <c r="D10" t="s">
+      <c r="H10" t="s">
         <v>108</v>
       </c>
-      <c r="E10" t="s">
-        <v>103</v>
-      </c>
-      <c r="F10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E11" t="s">
         <v>102</v>
       </c>
-      <c r="D11" s="12" t="s">
-        <v>112</v>
-      </c>
-      <c r="E11" t="s">
-        <v>103</v>
-      </c>
-      <c r="F11">
+      <c r="H11">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C12" t="s">
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="C14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D14" t="s">
+        <v>112</v>
+      </c>
+      <c r="E14" t="s">
         <v>102</v>
       </c>
-      <c r="D14" t="s">
-        <v>113</v>
-      </c>
-      <c r="E14" t="s">
-        <v>103</v>
-      </c>
-      <c r="F14">
+      <c r="H14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="C15" t="s">
+        <v>101</v>
+      </c>
+      <c r="D15" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" t="s">
         <v>102</v>
       </c>
-      <c r="D15" t="s">
-        <v>114</v>
-      </c>
-      <c r="E15" t="s">
-        <v>103</v>
-      </c>
-      <c r="F15">
+      <c r="H15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="C16" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" t="s">
+        <v>114</v>
+      </c>
+      <c r="E16" t="s">
         <v>102</v>
       </c>
-      <c r="D16" t="s">
-        <v>115</v>
-      </c>
-      <c r="E16" t="s">
-        <v>103</v>
-      </c>
-      <c r="F16">
+      <c r="H16">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="C17" t="s">
+        <v>101</v>
+      </c>
+      <c r="D17" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" t="s">
         <v>102</v>
       </c>
-      <c r="D17" t="s">
-        <v>116</v>
-      </c>
-      <c r="E17" t="s">
-        <v>103</v>
-      </c>
-      <c r="F17">
+      <c r="H17">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="C18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" t="s">
+        <v>116</v>
+      </c>
+      <c r="E18" t="s">
         <v>102</v>
       </c>
-      <c r="D18" t="s">
+      <c r="H18" t="s">
         <v>117</v>
       </c>
-      <c r="E18" t="s">
-        <v>103</v>
-      </c>
-      <c r="F18" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19" t="s">
         <v>102</v>
       </c>
-      <c r="D19" t="s">
-        <v>119</v>
-      </c>
-      <c r="E19" t="s">
-        <v>103</v>
-      </c>
-      <c r="F19" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C20" t="s">
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D21" t="s">
+        <v>124</v>
+      </c>
+      <c r="E21" t="s">
+        <v>123</v>
+      </c>
+      <c r="H21" t="s">
         <v>125</v>
       </c>
-      <c r="E21" t="s">
-        <v>124</v>
-      </c>
-      <c r="F21" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C22" t="s">
         <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C23" t="s">
         <v>19</v>
       </c>
       <c r="D23" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C24" t="s">
         <v>19</v>
       </c>
       <c r="D24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add link message type
Pair programmed with Jay
</commit_message>
<xml_diff>
--- a/resources/SPGeTTi_messages.xlsx
+++ b/resources/SPGeTTi_messages.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\761_ChatBot\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wlin8\Documents\761_ChatBot\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Welcome_Messages" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="146">
   <si>
     <t>Country</t>
   </si>
@@ -451,13 +451,28 @@
   </si>
   <si>
     <t>Message;Buttons;Store</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>Message;Link</t>
+  </si>
+  <si>
+    <t>Try these links for help</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://www.choicenotchance.org.nz/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -494,6 +509,14 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -537,10 +560,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -579,8 +603,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -892,20 +918,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -913,7 +939,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -921,7 +947,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -929,7 +955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -937,7 +963,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -945,7 +971,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -953,7 +979,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -961,7 +987,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -969,7 +995,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -977,7 +1003,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -985,7 +1011,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -993,7 +1019,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1008,20 +1034,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="40.7109375" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1035,7 +1061,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="36.75">
       <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
@@ -1049,7 +1075,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="36">
       <c r="A3" s="4" t="s">
         <v>25</v>
       </c>
@@ -1063,7 +1089,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="36.75">
       <c r="A4" s="5" t="s">
         <v>26</v>
       </c>
@@ -1077,7 +1103,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="48" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="48">
       <c r="A5" s="6" t="s">
         <v>28</v>
       </c>
@@ -1091,7 +1117,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="36">
       <c r="A6" s="6" t="s">
         <v>29</v>
       </c>
@@ -1105,7 +1131,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="36.75">
       <c r="A7" s="7" t="s">
         <v>30</v>
       </c>
@@ -1119,7 +1145,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="36.75">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -1133,7 +1159,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="36.75">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -1147,7 +1173,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="48.75">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -1161,7 +1187,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="36">
       <c r="A11" s="6" t="s">
         <v>34</v>
       </c>
@@ -1175,7 +1201,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="48" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="48">
       <c r="A12" s="4" t="s">
         <v>35</v>
       </c>
@@ -1189,7 +1215,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="24">
       <c r="A13" s="4" t="s">
         <v>36</v>
       </c>
@@ -1203,7 +1229,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="36">
       <c r="A14" s="4" t="s">
         <v>37</v>
       </c>
@@ -1217,7 +1243,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="48.75">
       <c r="A15" s="8" t="s">
         <v>39</v>
       </c>
@@ -1231,7 +1257,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="48.75">
       <c r="A16" s="5" t="s">
         <v>40</v>
       </c>
@@ -1245,7 +1271,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="36">
       <c r="A17" s="4" t="s">
         <v>41</v>
       </c>
@@ -1259,7 +1285,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="36">
       <c r="A18" s="4" t="s">
         <v>42</v>
       </c>
@@ -1273,7 +1299,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="48" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="48">
       <c r="A19" s="6" t="s">
         <v>43</v>
       </c>
@@ -1287,7 +1313,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="48" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="48">
       <c r="A20" s="6" t="s">
         <v>44</v>
       </c>
@@ -1301,7 +1327,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="36">
       <c r="A21" s="4" t="s">
         <v>45</v>
       </c>
@@ -1315,7 +1341,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="36.75">
       <c r="A22" s="5" t="s">
         <v>46</v>
       </c>
@@ -1329,7 +1355,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="36">
       <c r="A23" s="9" t="s">
         <v>47</v>
       </c>
@@ -1343,7 +1369,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="48.75">
       <c r="A24" s="7" t="s">
         <v>48</v>
       </c>
@@ -1357,7 +1383,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="36">
       <c r="A25" s="4" t="s">
         <v>49</v>
       </c>
@@ -1371,7 +1397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="48.75">
       <c r="A26" s="5" t="s">
         <v>50</v>
       </c>
@@ -1385,7 +1411,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="24">
       <c r="A27" s="4" t="s">
         <v>51</v>
       </c>
@@ -1399,7 +1425,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="24">
       <c r="A28" s="6" t="s">
         <v>52</v>
       </c>
@@ -1413,7 +1439,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="36">
       <c r="A29" s="4" t="s">
         <v>53</v>
       </c>
@@ -1427,7 +1453,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="36.75">
       <c r="A30" s="3" t="s">
         <v>54</v>
       </c>
@@ -1441,7 +1467,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="48.75">
       <c r="A31" s="5" t="s">
         <v>55</v>
       </c>
@@ -1455,7 +1481,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="48.75">
       <c r="A32" s="7" t="s">
         <v>56</v>
       </c>
@@ -1469,7 +1495,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="48.75">
       <c r="A33" s="5" t="s">
         <v>57</v>
       </c>
@@ -1483,7 +1509,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="48.75">
       <c r="A34" s="5" t="s">
         <v>58</v>
       </c>
@@ -1497,7 +1523,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="48.75">
       <c r="A35" s="5" t="s">
         <v>59</v>
       </c>
@@ -1511,7 +1537,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="36.75">
       <c r="A36" s="5" t="s">
         <v>60</v>
       </c>
@@ -1525,7 +1551,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="36.75">
       <c r="A37" s="3" t="s">
         <v>61</v>
       </c>
@@ -1539,7 +1565,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="36.75">
       <c r="A38" s="3" t="s">
         <v>62</v>
       </c>
@@ -1553,7 +1579,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="36">
       <c r="A39" s="4" t="s">
         <v>63</v>
       </c>
@@ -1567,7 +1593,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="36.75">
       <c r="A40" s="7" t="s">
         <v>64</v>
       </c>
@@ -1581,7 +1607,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="48" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="48">
       <c r="A41" s="6" t="s">
         <v>28</v>
       </c>
@@ -1595,7 +1621,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="36">
       <c r="A42" s="6" t="s">
         <v>65</v>
       </c>
@@ -1609,7 +1635,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="24.75">
       <c r="A43" s="8" t="s">
         <v>66</v>
       </c>
@@ -1623,7 +1649,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="48.75">
       <c r="A44" s="10" t="s">
         <v>67</v>
       </c>
@@ -1637,7 +1663,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="48.75">
       <c r="A45" s="7" t="s">
         <v>68</v>
       </c>
@@ -1651,7 +1677,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="24">
       <c r="A46" s="4" t="s">
         <v>69</v>
       </c>
@@ -1665,7 +1691,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="36.75">
       <c r="A47" s="8" t="s">
         <v>70</v>
       </c>
@@ -1679,7 +1705,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="24.75">
       <c r="A48" s="8" t="s">
         <v>71</v>
       </c>
@@ -1693,7 +1719,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="48" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="48">
       <c r="A49" s="6" t="s">
         <v>72</v>
       </c>
@@ -1707,7 +1733,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="36.75">
       <c r="A50" s="5" t="s">
         <v>73</v>
       </c>
@@ -1721,7 +1747,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="36.75">
       <c r="A51" s="5" t="s">
         <v>74</v>
       </c>
@@ -1735,7 +1761,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="25.5">
       <c r="A52" s="11" t="s">
         <v>75</v>
       </c>
@@ -1749,7 +1775,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="48" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="48">
       <c r="A53" s="6" t="s">
         <v>76</v>
       </c>
@@ -1769,23 +1795,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.28515625" customWidth="1"/>
+    <col min="6" max="8" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>85</v>
       </c>
@@ -1808,10 +1834,13 @@
         <v>132</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1827,11 +1856,11 @@
       <c r="E2" t="s">
         <v>102</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1847,11 +1876,11 @@
       <c r="E3" t="s">
         <v>102</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1867,11 +1896,11 @@
       <c r="E4" t="s">
         <v>102</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1888,29 +1917,49 @@
         <v>136</v>
       </c>
     </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" t="s">
+        <v>142</v>
+      </c>
+      <c r="D6" t="s">
+        <v>143</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>145</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H6" r:id="rId1" xr:uid="{7298C2B3-3669-499E-8DEF-2B60F3E85D91}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="4" max="4" width="97.42578125" customWidth="1"/>
-    <col min="5" max="7" width="31.85546875" customWidth="1"/>
+    <col min="5" max="8" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>85</v>
       </c>
@@ -1933,10 +1982,13 @@
         <v>132</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="45">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1951,11 +2003,12 @@
       </c>
       <c r="E2" s="12"/>
       <c r="G2" s="12"/>
-      <c r="H2" s="13">
+      <c r="H2" s="12"/>
+      <c r="I2" s="13">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1968,9 +2021,9 @@
       <c r="D3" t="s">
         <v>89</v>
       </c>
-      <c r="H3" s="13"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="13"/>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1986,11 +2039,11 @@
       <c r="F4" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="I4" s="13" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="30">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2006,9 +2059,10 @@
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
-      <c r="H5" s="13"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H5" s="12"/>
+      <c r="I5" s="13"/>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2024,11 +2078,11 @@
       <c r="E6" t="s">
         <v>102</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="I6" s="13" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="30">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2044,11 +2098,12 @@
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
-      <c r="H7" s="13">
+      <c r="H7" s="12"/>
+      <c r="I7" s="13">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2061,9 +2116,9 @@
       <c r="D8" t="s">
         <v>89</v>
       </c>
-      <c r="H8" s="13"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="13"/>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2078,9 +2133,10 @@
         <v>136</v>
       </c>
       <c r="G9" s="12"/>
-      <c r="H9" s="13"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H9" s="12"/>
+      <c r="I9" s="13"/>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2096,11 +2152,11 @@
       <c r="E10" t="s">
         <v>102</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="I10" s="13" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2116,11 +2172,11 @@
       <c r="E11" t="s">
         <v>102</v>
       </c>
-      <c r="H11" s="13">
+      <c r="I11" s="13">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2133,9 +2189,9 @@
       <c r="D12" t="s">
         <v>109</v>
       </c>
-      <c r="H12" s="13"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="13"/>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2148,9 +2204,9 @@
       <c r="D13" t="s">
         <v>110</v>
       </c>
-      <c r="H13" s="13"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="13"/>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2163,11 +2219,11 @@
       <c r="E14" t="s">
         <v>102</v>
       </c>
-      <c r="H14" s="13">
+      <c r="I14" s="13">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2180,11 +2236,11 @@
       <c r="E15" t="s">
         <v>102</v>
       </c>
-      <c r="H15" s="13">
+      <c r="I15" s="13">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2197,11 +2253,11 @@
       <c r="E16" t="s">
         <v>102</v>
       </c>
-      <c r="H16" s="13">
+      <c r="I16" s="13">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2214,11 +2270,11 @@
       <c r="E17" t="s">
         <v>102</v>
       </c>
-      <c r="H17" s="13">
+      <c r="I17" s="13">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2231,11 +2287,11 @@
       <c r="E18" t="s">
         <v>102</v>
       </c>
-      <c r="H18" s="13" t="s">
+      <c r="I18" s="13" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2251,11 +2307,11 @@
       <c r="E19" t="s">
         <v>102</v>
       </c>
-      <c r="H19" s="13" t="s">
+      <c r="I19" s="13" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2268,9 +2324,9 @@
       <c r="D20" t="s">
         <v>119</v>
       </c>
-      <c r="H20" s="13"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="13"/>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2286,11 +2342,11 @@
       <c r="E21" t="s">
         <v>123</v>
       </c>
-      <c r="H21" s="13" t="s">
+      <c r="I21" s="13" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2303,9 +2359,9 @@
       <c r="D22" t="s">
         <v>130</v>
       </c>
-      <c r="H22" s="13"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="13"/>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2319,7 +2375,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Added image message type
Pair programmed with Jay
</commit_message>
<xml_diff>
--- a/resources/SPGeTTi_messages.xlsx
+++ b/resources/SPGeTTi_messages.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\761_ChatBot\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wlin8\Documents\761_ChatBot\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Welcome_Messages" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="145">
   <si>
     <t>Country</t>
   </si>
@@ -451,13 +451,25 @@
   </si>
   <si>
     <t>Message;Buttons;Store</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>Message;Image</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>https://cdn.glitch.com/00ecfa44-32b0-4a79-a2a1-06d87dc60204%2Ftest_image.jpg?1506466359543</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -494,6 +506,14 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -537,10 +557,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -579,8 +600,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -892,20 +915,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -913,7 +936,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -921,7 +944,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -929,7 +952,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -937,7 +960,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -945,7 +968,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -953,7 +976,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -961,7 +984,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -969,7 +992,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -977,7 +1000,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -985,7 +1008,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -993,7 +1016,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1008,20 +1031,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="40.7109375" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1035,7 +1058,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="36.75">
       <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
@@ -1049,7 +1072,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="36">
       <c r="A3" s="4" t="s">
         <v>25</v>
       </c>
@@ -1063,7 +1086,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="36.75">
       <c r="A4" s="5" t="s">
         <v>26</v>
       </c>
@@ -1077,7 +1100,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="48" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="48">
       <c r="A5" s="6" t="s">
         <v>28</v>
       </c>
@@ -1091,7 +1114,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="36">
       <c r="A6" s="6" t="s">
         <v>29</v>
       </c>
@@ -1105,7 +1128,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="36.75">
       <c r="A7" s="7" t="s">
         <v>30</v>
       </c>
@@ -1119,7 +1142,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="36.75">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
@@ -1133,7 +1156,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="36.75">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -1147,7 +1170,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="48.75">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -1161,7 +1184,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="36">
       <c r="A11" s="6" t="s">
         <v>34</v>
       </c>
@@ -1175,7 +1198,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="48" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="48">
       <c r="A12" s="4" t="s">
         <v>35</v>
       </c>
@@ -1189,7 +1212,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="24">
       <c r="A13" s="4" t="s">
         <v>36</v>
       </c>
@@ -1203,7 +1226,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="36">
       <c r="A14" s="4" t="s">
         <v>37</v>
       </c>
@@ -1217,7 +1240,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="48.75">
       <c r="A15" s="8" t="s">
         <v>39</v>
       </c>
@@ -1231,7 +1254,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="48.75">
       <c r="A16" s="5" t="s">
         <v>40</v>
       </c>
@@ -1245,7 +1268,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="36">
       <c r="A17" s="4" t="s">
         <v>41</v>
       </c>
@@ -1259,7 +1282,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="36">
       <c r="A18" s="4" t="s">
         <v>42</v>
       </c>
@@ -1273,7 +1296,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="48" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="48">
       <c r="A19" s="6" t="s">
         <v>43</v>
       </c>
@@ -1287,7 +1310,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="48" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="48">
       <c r="A20" s="6" t="s">
         <v>44</v>
       </c>
@@ -1301,7 +1324,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="36">
       <c r="A21" s="4" t="s">
         <v>45</v>
       </c>
@@ -1315,7 +1338,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="36.75">
       <c r="A22" s="5" t="s">
         <v>46</v>
       </c>
@@ -1329,7 +1352,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="36">
       <c r="A23" s="9" t="s">
         <v>47</v>
       </c>
@@ -1343,7 +1366,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="48.75">
       <c r="A24" s="7" t="s">
         <v>48</v>
       </c>
@@ -1357,7 +1380,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="36">
       <c r="A25" s="4" t="s">
         <v>49</v>
       </c>
@@ -1371,7 +1394,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="48.75">
       <c r="A26" s="5" t="s">
         <v>50</v>
       </c>
@@ -1385,7 +1408,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="24">
       <c r="A27" s="4" t="s">
         <v>51</v>
       </c>
@@ -1399,7 +1422,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="24">
       <c r="A28" s="6" t="s">
         <v>52</v>
       </c>
@@ -1413,7 +1436,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="36">
       <c r="A29" s="4" t="s">
         <v>53</v>
       </c>
@@ -1427,7 +1450,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="36.75">
       <c r="A30" s="3" t="s">
         <v>54</v>
       </c>
@@ -1441,7 +1464,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="48.75">
       <c r="A31" s="5" t="s">
         <v>55</v>
       </c>
@@ -1455,7 +1478,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="48.75">
       <c r="A32" s="7" t="s">
         <v>56</v>
       </c>
@@ -1469,7 +1492,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="48.75">
       <c r="A33" s="5" t="s">
         <v>57</v>
       </c>
@@ -1483,7 +1506,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="48.75">
       <c r="A34" s="5" t="s">
         <v>58</v>
       </c>
@@ -1497,7 +1520,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="48.75">
       <c r="A35" s="5" t="s">
         <v>59</v>
       </c>
@@ -1511,7 +1534,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="36.75">
       <c r="A36" s="5" t="s">
         <v>60</v>
       </c>
@@ -1525,7 +1548,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="36.75">
       <c r="A37" s="3" t="s">
         <v>61</v>
       </c>
@@ -1539,7 +1562,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="36.75">
       <c r="A38" s="3" t="s">
         <v>62</v>
       </c>
@@ -1553,7 +1576,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="36">
       <c r="A39" s="4" t="s">
         <v>63</v>
       </c>
@@ -1567,7 +1590,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="36.75">
       <c r="A40" s="7" t="s">
         <v>64</v>
       </c>
@@ -1581,7 +1604,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="48" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="48">
       <c r="A41" s="6" t="s">
         <v>28</v>
       </c>
@@ -1595,7 +1618,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="36" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="36">
       <c r="A42" s="6" t="s">
         <v>65</v>
       </c>
@@ -1609,7 +1632,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="24.75">
       <c r="A43" s="8" t="s">
         <v>66</v>
       </c>
@@ -1623,7 +1646,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="48.75">
       <c r="A44" s="10" t="s">
         <v>67</v>
       </c>
@@ -1637,7 +1660,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="48.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="48.75">
       <c r="A45" s="7" t="s">
         <v>68</v>
       </c>
@@ -1651,7 +1674,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="24" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="24">
       <c r="A46" s="4" t="s">
         <v>69</v>
       </c>
@@ -1665,7 +1688,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="36.75">
       <c r="A47" s="8" t="s">
         <v>70</v>
       </c>
@@ -1679,7 +1702,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="24.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="24.75">
       <c r="A48" s="8" t="s">
         <v>71</v>
       </c>
@@ -1693,7 +1716,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="48" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="48">
       <c r="A49" s="6" t="s">
         <v>72</v>
       </c>
@@ -1707,7 +1730,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="36.75">
       <c r="A50" s="5" t="s">
         <v>73</v>
       </c>
@@ -1721,7 +1744,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="36.75">
       <c r="A51" s="5" t="s">
         <v>74</v>
       </c>
@@ -1735,7 +1758,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="25.5">
       <c r="A52" s="11" t="s">
         <v>75</v>
       </c>
@@ -1749,7 +1772,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="48" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="48">
       <c r="A53" s="6" t="s">
         <v>76</v>
       </c>
@@ -1769,23 +1792,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.28515625" customWidth="1"/>
+    <col min="6" max="8" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>85</v>
       </c>
@@ -1808,10 +1831,13 @@
         <v>132</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1827,11 +1853,11 @@
       <c r="E2" t="s">
         <v>102</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1847,11 +1873,11 @@
       <c r="E3" t="s">
         <v>102</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1867,11 +1893,11 @@
       <c r="E4" t="s">
         <v>102</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1888,21 +1914,38 @@
         <v>136</v>
       </c>
     </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" t="s">
+        <v>142</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>144</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H6" r:id="rId1" xr:uid="{1D824BA2-DA73-41CA-9861-C725E76CDEA2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
@@ -1910,7 +1953,7 @@
     <col min="5" max="7" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>85</v>
       </c>
@@ -1936,7 +1979,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="45">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1955,7 +1998,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1970,7 +2013,7 @@
       </c>
       <c r="H3" s="13"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1990,7 +2033,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="30">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2008,7 +2051,7 @@
       <c r="G5" s="12"/>
       <c r="H5" s="13"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2028,7 +2071,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="30">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2048,7 +2091,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2063,7 +2106,7 @@
       </c>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2080,7 +2123,7 @@
       <c r="G9" s="12"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2100,7 +2143,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2120,7 +2163,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2135,7 +2178,7 @@
       </c>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2150,7 +2193,7 @@
       </c>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2167,7 +2210,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>13</v>
       </c>
@@ -2184,7 +2227,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2201,7 +2244,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>15</v>
       </c>
@@ -2218,7 +2261,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2235,7 +2278,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2255,7 +2298,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2270,7 +2313,7 @@
       </c>
       <c r="H20" s="13"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2290,7 +2333,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2305,7 +2348,7 @@
       </c>
       <c r="H22" s="13"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2319,7 +2362,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="A24">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Converting messages to adaptive cards. Not complete yet
Pair programmed with Jay
</commit_message>
<xml_diff>
--- a/resources/SPGeTTi_messages.xlsx
+++ b/resources/SPGeTTi_messages.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="150">
   <si>
     <t>Country</t>
   </si>
@@ -463,6 +463,21 @@
   </si>
   <si>
     <t>https://cdn.glitch.com/00ecfa44-32b0-4a79-a2a1-06d87dc60204%2Ftest_image.jpg?1506466359543</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>Message;Link</t>
+  </si>
+  <si>
+    <t>Try look at these links for help</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://www.choicenotchance.org.nz/</t>
   </si>
 </sst>
 </file>
@@ -1793,10 +1808,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1805,10 +1820,10 @@
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="13.28515625" customWidth="1"/>
+    <col min="6" max="9" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>85</v>
       </c>
@@ -1834,10 +1849,13 @@
         <v>143</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1853,11 +1871,11 @@
       <c r="E2" t="s">
         <v>102</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1873,11 +1891,11 @@
       <c r="E3" t="s">
         <v>102</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1893,11 +1911,11 @@
       <c r="E4" t="s">
         <v>102</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1914,7 +1932,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1926,14 +1944,33 @@
       </c>
       <c r="H6" s="14" t="s">
         <v>144</v>
+      </c>
+      <c r="I6" s="14"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" t="s">
+        <v>147</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H6" r:id="rId1" xr:uid="{1D824BA2-DA73-41CA-9861-C725E76CDEA2}"/>
+    <hyperlink ref="I7" r:id="rId2" xr:uid="{7C5E6E95-844A-4D52-A5F4-7720AF538609}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add okay image and link card
-Pairprogrammed with Jay
</commit_message>
<xml_diff>
--- a/resources/SPGeTTi_messages.xlsx
+++ b/resources/SPGeTTi_messages.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="151">
   <si>
     <t>Country</t>
   </si>
@@ -462,25 +462,25 @@
     <t>Image</t>
   </si>
   <si>
-    <t>https://cdn.glitch.com/00ecfa44-32b0-4a79-a2a1-06d87dc60204%2Ftest_image.jpg?1506466359543</t>
-  </si>
-  <si>
     <t>link</t>
   </si>
   <si>
-    <t>Message;Link</t>
-  </si>
-  <si>
     <t>Try look at these links for help</t>
   </si>
   <si>
     <t>Link</t>
   </si>
   <si>
-    <t>https://www.choicenotchance.org.nz/</t>
-  </si>
-  <si>
     <t>Try looking at this image for help</t>
+  </si>
+  <si>
+    <t>Choice not Chance;https://www.choicenotchance.org.nz/</t>
+  </si>
+  <si>
+    <t>Message;Link;Image</t>
+  </si>
+  <si>
+    <t>https://cdn.glitch.com/00ecfa44-32b0-4a79-a2a1-06d87dc60204%2Ftest_image.jpg</t>
   </si>
 </sst>
 </file>
@@ -602,7 +602,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -644,6 +644,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1839,7 +1840,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1879,7 +1880,7 @@
         <v>143</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J1" s="14" t="s">
         <v>86</v>
@@ -1973,10 +1974,10 @@
         <v>142</v>
       </c>
       <c r="D6" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="H6" s="17" t="s">
         <v>150</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>144</v>
       </c>
       <c r="I6" s="16"/>
     </row>
@@ -1985,25 +1986,29 @@
         <v>5</v>
       </c>
       <c r="B7" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="D7" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>147</v>
+      <c r="H7" s="17" t="s">
+        <v>150</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="H6" r:id="rId1" xr:uid="{1D824BA2-DA73-41CA-9861-C725E76CDEA2}"/>
-    <hyperlink ref="I7" r:id="rId2" xr:uid="{7C5E6E95-844A-4D52-A5F4-7720AF538609}"/>
+    <hyperlink ref="I7" r:id="rId2" display="https://www.choicenotchance.org.nz/" xr:uid="{7C5E6E95-844A-4D52-A5F4-7720AF538609}"/>
+    <hyperlink ref="H7" r:id="rId3" xr:uid="{4E52B34F-D038-4592-A603-6D2B82D70F36}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -2053,7 +2058,7 @@
         <v>143</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
Add randomisation of messages from pool
Pairprogrammed with Jay
</commit_message>
<xml_diff>
--- a/resources/SPGeTTi_messages.xlsx
+++ b/resources/SPGeTTi_messages.xlsx
@@ -291,9 +291,6 @@
     <t>Follow Ups</t>
   </si>
   <si>
-    <t>Need help setting some goals?</t>
-  </si>
-  <si>
     <t>0;1</t>
   </si>
   <si>
@@ -315,9 +312,6 @@
     <t>Great, there's lots of benefits by not gambling.  Some benefits are getting out of debt, improving relationships, feeling healthier and less stressed, feeling better about yourself.  What do you see as your benefits by stopping gambling?</t>
   </si>
   <si>
-    <t>Great, here are some quick tips to start this journey:  Avoid tempting environments; Limit access to finances; Find healthier activities to do</t>
-  </si>
-  <si>
     <t>Try to limit how many days you go gambling, or set a maximum amount you can spend.  Take some time now to write down what you want to achieve</t>
   </si>
   <si>
@@ -481,6 +475,12 @@
   </si>
   <si>
     <t>https://cdn.glitch.com/00ecfa44-32b0-4a79-a2a1-06d87dc60204%2Ftest_image.jpg</t>
+  </si>
+  <si>
+    <t>Great, here are some quick tips to start this journey:  Avoid tempting environments, Limit access to finances, Find healthier activities to do</t>
+  </si>
+  <si>
+    <t>Need help setting some goals?;Would you like to set some goals?; Do you want to set some goals?</t>
   </si>
 </sst>
 </file>
@@ -602,7 +602,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -644,7 +644,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1840,7 +1839,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1862,25 +1861,25 @@
         <v>84</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>19</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F1" s="14" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="J1" s="14" t="s">
         <v>86</v>
@@ -1891,19 +1890,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D2" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="J2" s="15" t="s">
         <v>87</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1911,19 +1910,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="J3" s="15" t="s">
         <v>104</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="J3" s="15" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1931,19 +1930,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="J4" s="15" t="s">
         <v>120</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1951,16 +1950,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="G5" s="15" t="s">
         <v>134</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>135</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1968,16 +1967,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>150</v>
+        <v>145</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>148</v>
       </c>
       <c r="I6" s="16"/>
     </row>
@@ -1986,19 +1985,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>150</v>
+        <v>143</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>148</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2017,7 +2016,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2040,25 +2039,25 @@
         <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>86</v>
@@ -2069,13 +2068,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E2" s="12"/>
       <c r="G2" s="12"/>
@@ -2090,13 +2089,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J3" s="13"/>
     </row>
@@ -2105,19 +2104,19 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="J4" s="13" t="s">
         <v>90</v>
-      </c>
-      <c r="E4" t="s">
-        <v>102</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2125,13 +2124,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>95</v>
+        <v>149</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
@@ -2145,19 +2144,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" t="s">
+        <v>100</v>
+      </c>
+      <c r="J6" s="13" t="s">
         <v>92</v>
-      </c>
-      <c r="E6" t="s">
-        <v>102</v>
-      </c>
-      <c r="J6" s="13" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -2165,13 +2164,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
@@ -2187,13 +2186,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J8" s="13"/>
     </row>
@@ -2202,14 +2201,14 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9" s="12" t="s">
         <v>137</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>139</v>
       </c>
       <c r="E9" s="12"/>
       <c r="F9" s="12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
@@ -2221,19 +2220,19 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D10" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2241,16 +2240,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J11" s="13">
         <v>12</v>
@@ -2261,13 +2260,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C12" t="s">
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J12" s="13"/>
     </row>
@@ -2276,13 +2275,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J13" s="13"/>
     </row>
@@ -2291,13 +2290,13 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D14" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E14" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J14" s="13">
         <v>13</v>
@@ -2308,13 +2307,13 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J15" s="13">
         <v>14</v>
@@ -2325,13 +2324,13 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E16" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J16" s="13">
         <v>15</v>
@@ -2342,13 +2341,13 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D17" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J17" s="13">
         <v>16</v>
@@ -2359,16 +2358,16 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -2376,19 +2375,19 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D19" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -2396,13 +2395,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C20" t="s">
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="J20" s="13"/>
     </row>
@@ -2411,19 +2410,19 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D21" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E21" t="s">
+        <v>121</v>
+      </c>
+      <c r="J21" s="13" t="s">
         <v>123</v>
-      </c>
-      <c r="J21" s="13" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -2431,13 +2430,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C22" t="s">
         <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J22" s="13"/>
     </row>
@@ -2446,13 +2445,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C23" t="s">
         <v>19</v>
       </c>
       <c r="D23" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -2460,13 +2459,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C24" t="s">
         <v>19</v>
       </c>
       <c r="D24" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Replace adaptive with Hero cards
Hero cards are better formatted in FB.

Pairprogrammed with Jay
</commit_message>
<xml_diff>
--- a/resources/SPGeTTi_messages.xlsx
+++ b/resources/SPGeTTi_messages.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Welcome_Messages" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="150">
   <si>
     <t>Country</t>
   </si>
@@ -447,47 +447,44 @@
     <t>Message;Buttons;Store</t>
   </si>
   <si>
-    <t>image</t>
-  </si>
-  <si>
-    <t>Message;Image</t>
-  </si>
-  <si>
     <t>Image</t>
   </si>
   <si>
     <t>link</t>
   </si>
   <si>
-    <t>Try look at these links for help</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
-    <t>Try looking at this image for help</t>
-  </si>
-  <si>
-    <t>Choice not Chance;https://www.choicenotchance.org.nz/</t>
-  </si>
-  <si>
-    <t>Message;Link;Image</t>
+    <t>Great, here are some quick tips to start this journey:  Avoid tempting environments, Limit access to finances, Find healthier activities to do</t>
+  </si>
+  <si>
+    <t>Need help setting some goals?;Would you like to set some goals?; Do you want to set some goals?</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Need more help?</t>
+  </si>
+  <si>
+    <t>Try look at this link for more help.</t>
+  </si>
+  <si>
+    <t>Choice not Chance;https://www.choicenotchance.org.nz/;Youtube;https://www.youtube.com/</t>
   </si>
   <si>
     <t>https://cdn.glitch.com/00ecfa44-32b0-4a79-a2a1-06d87dc60204%2Ftest_image.jpg</t>
   </si>
   <si>
-    <t>Great, here are some quick tips to start this journey:  Avoid tempting environments, Limit access to finances, Find healthier activities to do</t>
-  </si>
-  <si>
-    <t>Need help setting some goals?;Would you like to set some goals?; Do you want to set some goals?</t>
+    <t>Message;Link;Image;Title</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -532,6 +529,21 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -602,7 +614,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -635,15 +647,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1836,635 +1850,631 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="15"/>
-    <col min="2" max="2" width="9.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="13.28515625" style="15" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="15"/>
+    <col min="1" max="1" width="9.140625" style="17"/>
+    <col min="2" max="2" width="9.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="13.28515625" style="17" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="I1" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="J1" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="K1" s="16" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="17">
         <v>0</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="E2" s="15" t="s">
+      <c r="D2" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="K2" s="17" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="17">
         <v>1</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="K3" s="17" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
         <v>2</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="17" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="K4" s="17" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="17">
         <v>3</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="17" t="s">
         <v>131</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="17" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
         <v>4</v>
       </c>
-      <c r="B6" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="C6" s="15" t="s">
+      <c r="B6" s="17" t="s">
         <v>140</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="C6" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="J6" s="18" t="s">
         <v>145</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="I6" s="16"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="15">
-        <v>5</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>142</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>146</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H6" r:id="rId1" xr:uid="{1D824BA2-DA73-41CA-9861-C725E76CDEA2}"/>
-    <hyperlink ref="I7" r:id="rId2" display="https://www.choicenotchance.org.nz/" xr:uid="{7C5E6E95-844A-4D52-A5F4-7720AF538609}"/>
-    <hyperlink ref="H7" r:id="rId3" xr:uid="{4E52B34F-D038-4592-A603-6D2B82D70F36}"/>
+    <hyperlink ref="I6" r:id="rId1" display="https://www.choicenotchance.org.nz/" xr:uid="{7C5E6E95-844A-4D52-A5F4-7720AF538609}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="97.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="13"/>
+    <col min="2" max="2" width="19.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="97.42578125" style="13" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5" style="13" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="I1" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="12" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="13">
+      <c r="E2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="15">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="J3" s="13"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="K3" s="15"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="K4" s="15" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="13"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="D5" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="J6" s="13" t="s">
+      <c r="K6" s="15" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="13">
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="15">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="J8" s="13"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="K8" s="15"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12" t="s">
+      <c r="E9" s="14"/>
+      <c r="F9" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="13"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="15"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="K10" s="15" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="J11" s="13">
+      <c r="K11" s="15">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="J12" s="13"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="K12" s="15"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="13">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="J13" s="13"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="K13" s="15"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
         <v>12</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="J14" s="13">
+      <c r="K14" s="15">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="13">
         <v>13</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="J15" s="13">
+      <c r="K15" s="15">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
         <v>14</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="J16" s="13">
+      <c r="K16" s="15">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="13">
         <v>15</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="J17" s="13">
+      <c r="K17" s="15">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="13">
         <v>16</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="J18" s="13" t="s">
+      <c r="K18" s="15" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="13">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="J19" s="13" t="s">
+      <c r="K19" s="15" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="13">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="J20" s="13"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="K20" s="15"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="13">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="J21" s="13" t="s">
+      <c r="K21" s="15" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="13">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="J22" s="13"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="K22" s="15"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="13">
         <v>21</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="13">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="13" t="s">
         <v>127</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add presentation for presenting
Pair programmed with JAY
</commit_message>
<xml_diff>
--- a/resources/SPGeTTi_messages.xlsx
+++ b/resources/SPGeTTi_messages.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="179">
   <si>
     <t>Country</t>
   </si>
@@ -333,9 +333,6 @@
     <t>Yes;No</t>
   </si>
   <si>
-    <t>goals</t>
-  </si>
-  <si>
     <t>problems</t>
   </si>
   <si>
@@ -348,12 +345,6 @@
     <t>You are not alone. Do you want to talk to someone?</t>
   </si>
   <si>
-    <t>10;11</t>
-  </si>
-  <si>
-    <t>You can phone a friend, call the Gambling Helpline 0800 654 655 or text 8006 for more information</t>
-  </si>
-  <si>
     <t>If you want more information, you can go to choicenotchance.org.nz</t>
   </si>
   <si>
@@ -381,9 +372,6 @@
     <t>It looks like gambling is hurting you and maybe those you care about. Do you want to talk to someone about it?</t>
   </si>
   <si>
-    <t>Okay that's great! If you want more information, you can go to choicenotchance.org.nz</t>
-  </si>
-  <si>
     <t>stressed</t>
   </si>
   <si>
@@ -408,9 +396,6 @@
     <t>outdoors</t>
   </si>
   <si>
-    <t>Why don't you invite your friends over for dinner? You find some recipes at myfamily.kiwi/foods</t>
-  </si>
-  <si>
     <t>You can go for a walk, visit a museum or gallery with your friends or family. Going to a nearby park is also a fun thing to do!</t>
   </si>
   <si>
@@ -478,6 +463,108 @@
   </si>
   <si>
     <t>Message;Link;Image;Title</t>
+  </si>
+  <si>
+    <t>yes;no</t>
+  </si>
+  <si>
+    <t>Title;Message;Image;Link</t>
+  </si>
+  <si>
+    <t>If you want more information, you can go to choicenotchance</t>
+  </si>
+  <si>
+    <t>Want more?</t>
+  </si>
+  <si>
+    <t>https://www.hetaumata.co.nz/sites/default/files/pictures/CnC%20FINAL%20LOGO_Strap%20CMYK_ver_no%20grad.jpg</t>
+  </si>
+  <si>
+    <t>10;18</t>
+  </si>
+  <si>
+    <t>http://www.wrh-global-americas.com/data/docs/en/5082/Service-Titelbild-1.jpg?variant=3439&amp;v=1.0</t>
+  </si>
+  <si>
+    <t>Message;Image;Title</t>
+  </si>
+  <si>
+    <t>Call for help</t>
+  </si>
+  <si>
+    <t>Call the Gambling Helpline 0800 654 655 or text 8006 for more info</t>
+  </si>
+  <si>
+    <t>myfamily.kiwi/foods</t>
+  </si>
+  <si>
+    <t>Why don't you invite your friends over for dinner? Use some new recipes!</t>
+  </si>
+  <si>
+    <t>http://images.contentful.com/6fpp5r5onj5r/3gXKQiIFckYc6oSY2W6eaG/0f0ea7f77efa02c58ece0d5b39f84a3b/Thai_chicken_salad.jpg?w=485</t>
+  </si>
+  <si>
+    <t>Message;Link;Title;Image</t>
+  </si>
+  <si>
+    <t>set goals</t>
+  </si>
+  <si>
+    <t>present</t>
+  </si>
+  <si>
+    <t>Hi, I'm Spgetti Bot!</t>
+  </si>
+  <si>
+    <t>Here to help with your problemos!</t>
+  </si>
+  <si>
+    <t>https://d2gg9evh47fn9z.cloudfront.net/thumb_COLOURBOX6978004.jpg</t>
+  </si>
+  <si>
+    <t>I'm a super multi-functional bot to help with your gambling addictions!  I can send you messages to see how you're doing, give you helpful links, and I'm super smart so I can even hold a real conversation!</t>
+  </si>
+  <si>
+    <t>We're holding a conversation now silly! ;P</t>
+  </si>
+  <si>
+    <t>I can remember what we've talked about so I can remind you later too!</t>
+  </si>
+  <si>
+    <t>Sure!  I'll remember that foreveeeeer.  Y'know, I can send fancy messages with images a links too!</t>
+  </si>
+  <si>
+    <t>This is one of my favs!</t>
+  </si>
+  <si>
+    <t>I sure do!  But aren’t you forgetting something?</t>
+  </si>
+  <si>
+    <t>Click me!;Or me!</t>
+  </si>
+  <si>
+    <t>You asked me to remember: [Goals].  You're welcome for the reminder!</t>
+  </si>
+  <si>
+    <t>I think that's all.  But I can be easily extended by spreadsheets whenever you want!</t>
+  </si>
+  <si>
+    <t>See ya!</t>
+  </si>
+  <si>
+    <t>That's all for now!</t>
+  </si>
+  <si>
+    <t>Message;Image;Title;Link</t>
+  </si>
+  <si>
+    <t>Goodbye;https://youtu.be/SW-BU6keEUw?t=4s</t>
+  </si>
+  <si>
+    <t>Choice Not Chance;choicenotchance.org.nz</t>
+  </si>
+  <si>
+    <t>Choice not Chance;https://www.choicenotchance.org.nz/</t>
   </si>
 </sst>
 </file>
@@ -614,7 +701,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -655,9 +742,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1850,173 +1939,197 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="17"/>
-    <col min="2" max="2" width="9.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="10" width="13.28515625" style="17" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="17"/>
+    <col min="1" max="1" width="9.140625" style="18"/>
+    <col min="2" max="2" width="9.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="13.28515625" style="18" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="G1" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="I1" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="J1" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="18">
+        <v>0</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="18">
+        <v>1</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="18">
+        <v>2</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="18">
+        <v>3</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="G5" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="G1" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="I1" s="16" t="s">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="18">
+        <v>4</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="J1" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="K1" s="16" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="17">
-        <v>0</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="D2" s="17" t="s">
+      <c r="H6" s="20" t="s">
         <v>143</v>
       </c>
-      <c r="E2" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="K2" s="17" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="17">
-        <v>1</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="K3" s="17" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
-        <v>2</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="K4" s="17" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
-        <v>3</v>
-      </c>
-      <c r="B5" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
-        <v>4</v>
-      </c>
-      <c r="B6" s="17" t="s">
+      <c r="I6" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="J6" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="I6" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="J6" s="18" t="s">
-        <v>145</v>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="18">
+        <v>5</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="K7" s="18">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I6" r:id="rId1" display="https://www.choicenotchance.org.nz/" xr:uid="{7C5E6E95-844A-4D52-A5F4-7720AF538609}"/>
+    <hyperlink ref="H6" r:id="rId2" xr:uid="{F16A2FEE-03E4-44CE-BE60-D9C73BC273E3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2051,19 +2164,19 @@
         <v>98</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H1" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="J1" s="12" t="s">
         <v>139</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>144</v>
       </c>
       <c r="K1" s="12" t="s">
         <v>86</v>
@@ -2111,7 +2224,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>89</v>
@@ -2120,7 +2233,7 @@
         <v>100</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="K4" s="15" t="s">
         <v>90</v>
@@ -2137,7 +2250,7 @@
         <v>19</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
@@ -2210,14 +2323,14 @@
         <v>7</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E9" s="14"/>
       <c r="F9" s="14" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -2236,13 +2349,13 @@
         <v>99</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>100</v>
       </c>
       <c r="K10" s="15" t="s">
-        <v>106</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -2256,7 +2369,7 @@
         <v>99</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E11" s="13" t="s">
         <v>100</v>
@@ -2273,10 +2386,16 @@
         <v>95</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>19</v>
+        <v>152</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>107</v>
+        <v>154</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>153</v>
       </c>
       <c r="K12" s="15"/>
     </row>
@@ -2291,7 +2410,7 @@
         <v>19</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="K13" s="15"/>
     </row>
@@ -2299,11 +2418,14 @@
       <c r="A14" s="13">
         <v>12</v>
       </c>
+      <c r="B14" s="13" t="s">
+        <v>145</v>
+      </c>
       <c r="C14" s="13" t="s">
         <v>99</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>100</v>
@@ -2316,11 +2438,14 @@
       <c r="A15" s="13">
         <v>13</v>
       </c>
+      <c r="B15" s="13" t="s">
+        <v>145</v>
+      </c>
       <c r="C15" s="13" t="s">
         <v>99</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>100</v>
@@ -2333,11 +2458,14 @@
       <c r="A16" s="13">
         <v>14</v>
       </c>
+      <c r="B16" s="13" t="s">
+        <v>145</v>
+      </c>
       <c r="C16" s="13" t="s">
         <v>99</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>100</v>
@@ -2350,11 +2478,14 @@
       <c r="A17" s="13">
         <v>15</v>
       </c>
+      <c r="B17" s="13" t="s">
+        <v>145</v>
+      </c>
       <c r="C17" s="13" t="s">
         <v>99</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E17" s="13" t="s">
         <v>100</v>
@@ -2367,17 +2498,20 @@
       <c r="A18" s="13">
         <v>16</v>
       </c>
+      <c r="B18" s="13" t="s">
+        <v>145</v>
+      </c>
       <c r="C18" s="13" t="s">
         <v>99</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E18" s="13" t="s">
         <v>100</v>
       </c>
       <c r="K18" s="15" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -2391,13 +2525,13 @@
         <v>99</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E19" s="13" t="s">
         <v>100</v>
       </c>
       <c r="K19" s="15" t="s">
-        <v>106</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -2408,10 +2542,19 @@
         <v>96</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>19</v>
+        <v>146</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>117</v>
+        <v>147</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="J20" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="K20" s="15"/>
     </row>
@@ -2426,13 +2569,13 @@
         <v>99</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="K21" s="15" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -2446,7 +2589,7 @@
         <v>19</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="K22" s="15"/>
     </row>
@@ -2455,13 +2598,19 @@
         <v>21</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>19</v>
+        <v>158</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>126</v>
+        <v>156</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -2469,13 +2618,188 @@
         <v>22</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="13">
+        <v>23</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="K25" s="18">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="13">
+        <v>24</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="K26" s="13">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="13">
+        <v>25</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="K27" s="13">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="13">
+        <v>26</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="K28" s="13">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="13">
+        <v>27</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="K29" s="16">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="13">
+        <v>28</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="I30" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="J30" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="K30" s="16">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="13">
+        <v>29</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="G31" s="16"/>
+      <c r="K31" s="16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="16">
+        <v>30</v>
+      </c>
+      <c r="C32" s="16" t="s">
         <v>127</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="G32" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="K32" s="16">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="16">
+        <v>31</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="K33" s="16">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="16">
+        <v>32</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="I34" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="J34" s="16" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>